<commit_message>
some pics and tables and nad
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\presw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mipClanok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11395AEC-39BD-44EF-B021-E4892208B9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B52865C-A4FB-4513-96F9-79BD96118DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="2472" windowWidth="17280" windowHeight="8880" xr2:uid="{1EE6E2DB-9F10-439B-AA82-959FCA646E73}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1EE6E2DB-9F10-439B-AA82-959FCA646E73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="zaujem" sheetId="2" r:id="rId2"/>
-    <sheet name="vykon" sheetId="3" r:id="rId3"/>
+    <sheet name="skusenosti" sheetId="4" r:id="rId2"/>
+    <sheet name="zaujem" sheetId="2" r:id="rId3"/>
+    <sheet name="vykon" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Skupina Habitica Pre</t>
   </si>
@@ -50,17 +51,27 @@
     <t>Kontrolná skupina Pre</t>
   </si>
   <si>
-    <t>Hodnotený osobný záujem o dosiahnutie svojho cieľa</t>
+    <t>Ako hodnotíte svoje doterajšie skúsenosti so snahou dosiahnuť tento cieľ?</t>
   </si>
   <si>
-    <t>Hodnotenie výkonu</t>
+    <t>Ako hodnotíte svoj doterajší výkon v snahe dosiahnuť tento cieľ?</t>
+  </si>
+  <si>
+    <t>Aký osobný záujem máte na dosiahnutí tohto cieľa?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -100,20 +111,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -124,12 +127,20 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -179,7 +190,641 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Hodnotený osobný záujem o dosiahnutie svojho cieľa</a:t>
+              <a:t>Ako hodnotíte svoje doterajšie skúsenosti so snahou dosiahnuť tento cieľ?</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Skupina Habitica Pre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$23:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2BE7-4C50-9D87-BDDB640BB7FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kontrolná skupina Pre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$23:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$23:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2BE7-4C50-9D87-BDDB640BB7FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Skupina Habitica Post</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$23:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$23:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2BE7-4C50-9D87-BDDB640BB7FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kontrolná skupina Post</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$23:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$23:$E$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2BE7-4C50-9D87-BDDB640BB7FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="862300751"/>
+        <c:axId val="865656127"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="862300751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="865656127"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="865656127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="862300751"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-UA"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Aký osobný záujem máte na dosiahnutí tohto cieľa?</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -778,7 +1423,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -813,7 +1458,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Hodnotenie výkonu</a:t>
+              <a:t>Ako hodnotíte svoj doterajší výkon v snahe dosiahnuť tento cieľ?</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1492,6 +2137,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2498,7 +3183,521 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{46ABBC81-9744-4858-B53C-8D74CED36194}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="88" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E78737A7-4BEB-489C-AF5A-E27D669CD0F7}">
   <sheetPr/>
   <sheetViews>
@@ -2509,7 +3708,7 @@
 </chartsheet>
 </file>
 
-<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{6AA750DB-EF53-48BB-AF1E-50AE10431F5D}">
   <sheetPr/>
   <sheetViews>
@@ -2521,6 +3720,39 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9291205" cy="6070023"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A5DA35A-F834-4ADA-853F-10BE3ACD750A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -2553,7 +3785,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -2883,10 +4115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DFBEA9-E70B-4F4C-98F2-28944EDD3A0D}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2895,18 +4127,20 @@
     <col min="2" max="3" width="10.77734375" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2921,7 +4155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2938,7 +4172,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2955,7 +4189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2972,7 +4206,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2989,7 +4223,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3006,7 +4240,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3023,7 +4257,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3040,21 +4274,22 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>0</v>
@@ -3069,7 +4304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -3086,7 +4321,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -3103,7 +4338,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -3120,7 +4355,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -3137,7 +4372,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>5</v>
       </c>
@@ -3154,7 +4389,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>6</v>
       </c>
@@ -3171,7 +4406,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -3188,16 +4423,161 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="C24" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>3</v>
+      </c>
+      <c r="B25" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>4</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>5</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.26</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>6</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>7</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0.15</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A11:E11"/>
+  <mergeCells count="3">
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>